<commit_message>
Add cv79 to features spreadsheet [nobuild]
</commit_message>
<xml_diff>
--- a/source/opentype/featureinfo.xlsx
+++ b/source/opentype/featureinfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victor/Work/Roman/Charis/font-charis/source/opentype/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E83967F-02AE-2F4E-ADAD-AFFD0ACDB93A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD8BE959-0803-7D41-9570-59FBF6BB5E32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15840" yWindow="480" windowWidth="47080" windowHeight="42720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="512">
   <si>
     <t>0071 02A0 A757 A759</t>
   </si>
@@ -2218,6 +2218,12 @@
   </si>
   <si>
     <t>004A 0134 0248 1D0A 1D36 A7B2</t>
+  </si>
+  <si>
+    <t>Kayan diacritics</t>
+  </si>
+  <si>
+    <t>cv79</t>
   </si>
 </sst>
 </file>
@@ -2843,6 +2849,54 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -2860,54 +2914,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3404,13 +3410,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O62"/>
+  <dimension ref="A1:O63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L1" sqref="L1:L1048576"/>
+      <selection pane="bottomRight" activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3430,21 +3436,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="79" t="s">
         <v>232</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="65"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="81"/>
       <c r="F1" s="56" t="s">
         <v>420</v>
       </c>
-      <c r="G1" s="60" t="s">
+      <c r="G1" s="76" t="s">
         <v>326</v>
       </c>
-      <c r="H1" s="61"/>
-      <c r="I1" s="62"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="78"/>
       <c r="J1" s="7" t="s">
         <v>233</v>
       </c>
@@ -3513,7 +3519,7 @@
       <c r="F3" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="G3" s="77" t="s">
+      <c r="G3" s="60" t="s">
         <v>136</v>
       </c>
       <c r="H3" s="22">
@@ -3525,7 +3531,7 @@
       <c r="K3" s="24" t="s">
         <v>168</v>
       </c>
-      <c r="L3" s="77" t="s">
+      <c r="L3" s="60" t="s">
         <v>426</v>
       </c>
       <c r="M3" s="24" t="s">
@@ -3551,7 +3557,7 @@
       <c r="F4" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="G4" s="77" t="s">
+      <c r="G4" s="60" t="s">
         <v>294</v>
       </c>
       <c r="J4" s="12" t="s">
@@ -3560,7 +3566,7 @@
       <c r="K4" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="L4" s="77" t="s">
+      <c r="L4" s="60" t="s">
         <v>427</v>
       </c>
       <c r="M4" s="24" t="s">
@@ -3586,7 +3592,7 @@
       <c r="F5" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="G5" s="77" t="s">
+      <c r="G5" s="60" t="s">
         <v>421</v>
       </c>
       <c r="J5" s="9" t="s">
@@ -3595,7 +3601,7 @@
       <c r="K5" s="24" t="s">
         <v>170</v>
       </c>
-      <c r="L5" s="77" t="s">
+      <c r="L5" s="60" t="s">
         <v>428</v>
       </c>
       <c r="M5" s="24" t="s">
@@ -3621,7 +3627,7 @@
       <c r="F6" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="G6" s="77" t="s">
+      <c r="G6" s="60" t="s">
         <v>422</v>
       </c>
       <c r="J6" s="9" t="s">
@@ -3630,7 +3636,7 @@
       <c r="K6" s="24" t="s">
         <v>171</v>
       </c>
-      <c r="L6" s="77" t="s">
+      <c r="L6" s="60" t="s">
         <v>429</v>
       </c>
       <c r="M6" s="24" t="s">
@@ -3656,7 +3662,7 @@
       <c r="F7" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="G7" s="77" t="s">
+      <c r="G7" s="60" t="s">
         <v>423</v>
       </c>
       <c r="J7" s="9" t="s">
@@ -3665,7 +3671,7 @@
       <c r="K7" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="L7" s="77" t="s">
+      <c r="L7" s="60" t="s">
         <v>430</v>
       </c>
       <c r="M7" s="24" t="s">
@@ -3691,7 +3697,7 @@
       <c r="F8" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="G8" s="77" t="s">
+      <c r="G8" s="60" t="s">
         <v>424</v>
       </c>
       <c r="J8" s="9" t="s">
@@ -3700,7 +3706,7 @@
       <c r="K8" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="L8" s="77" t="s">
+      <c r="L8" s="60" t="s">
         <v>431</v>
       </c>
       <c r="M8" s="24" t="s">
@@ -3729,7 +3735,7 @@
       <c r="F9" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="G9" s="77" t="s">
+      <c r="G9" s="60" t="s">
         <v>229</v>
       </c>
       <c r="J9" s="9" t="s">
@@ -3738,7 +3744,7 @@
       <c r="K9" s="24" t="s">
         <v>174</v>
       </c>
-      <c r="L9" s="77" t="s">
+      <c r="L9" s="60" t="s">
         <v>432</v>
       </c>
       <c r="M9" s="24" t="s">
@@ -3764,7 +3770,7 @@
       <c r="F10" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="G10" s="77" t="s">
+      <c r="G10" s="60" t="s">
         <v>425</v>
       </c>
       <c r="J10" s="10" t="s">
@@ -3773,7 +3779,7 @@
       <c r="K10" s="24" t="s">
         <v>175</v>
       </c>
-      <c r="L10" s="77" t="s">
+      <c r="L10" s="60" t="s">
         <v>433</v>
       </c>
       <c r="M10" s="24" t="s">
@@ -3781,36 +3787,36 @@
       </c>
     </row>
     <row r="11" spans="1:15" s="14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="68" t="s">
+      <c r="A11" s="67" t="s">
         <v>241</v>
       </c>
       <c r="B11" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="70">
+      <c r="C11" s="69">
         <v>1032</v>
       </c>
       <c r="D11" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="72" t="s">
+      <c r="E11" s="71" t="s">
         <v>259</v>
       </c>
-      <c r="F11" s="76" t="s">
+      <c r="F11" s="75" t="s">
         <v>229</v>
       </c>
-      <c r="G11" s="74" t="s">
+      <c r="G11" s="73" t="s">
         <v>229</v>
       </c>
       <c r="H11" s="25"/>
       <c r="I11" s="26"/>
-      <c r="J11" s="66" t="s">
+      <c r="J11" s="65" t="s">
         <v>244</v>
       </c>
       <c r="K11" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="L11" s="77" t="s">
+      <c r="L11" s="60" t="s">
         <v>435</v>
       </c>
       <c r="M11" s="24" t="s">
@@ -3818,18 +3824,18 @@
       </c>
     </row>
     <row r="12" spans="1:15" s="14" customFormat="1" ht="85" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="69"/>
+      <c r="A12" s="68"/>
       <c r="B12" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="71"/>
+      <c r="C12" s="70"/>
       <c r="D12" s="42"/>
-      <c r="E12" s="73"/>
-      <c r="F12" s="69"/>
-      <c r="G12" s="75"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="74"/>
       <c r="H12" s="54"/>
       <c r="I12" s="27"/>
-      <c r="J12" s="67"/>
+      <c r="J12" s="66"/>
     </row>
     <row r="13" spans="1:15" ht="43" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" s="57" t="s">
@@ -3859,7 +3865,7 @@
       <c r="K13" s="24" t="s">
         <v>177</v>
       </c>
-      <c r="L13" s="77" t="s">
+      <c r="L13" s="60" t="s">
         <v>436</v>
       </c>
       <c r="M13" s="24" t="s">
@@ -3894,7 +3900,7 @@
       <c r="K14" s="24" t="s">
         <v>178</v>
       </c>
-      <c r="L14" s="77" t="s">
+      <c r="L14" s="60" t="s">
         <v>437</v>
       </c>
       <c r="M14" s="24" t="s">
@@ -3929,7 +3935,7 @@
       <c r="K15" s="24" t="s">
         <v>179</v>
       </c>
-      <c r="L15" s="77" t="s">
+      <c r="L15" s="60" t="s">
         <v>438</v>
       </c>
       <c r="M15" s="24" t="s">
@@ -3964,7 +3970,7 @@
       <c r="K16" s="24" t="s">
         <v>180</v>
       </c>
-      <c r="L16" s="77" t="s">
+      <c r="L16" s="60" t="s">
         <v>439</v>
       </c>
       <c r="M16" s="24" t="s">
@@ -3999,7 +4005,7 @@
       <c r="K17" s="24" t="s">
         <v>181</v>
       </c>
-      <c r="L17" s="77" t="s">
+      <c r="L17" s="60" t="s">
         <v>440</v>
       </c>
       <c r="M17" s="24" t="s">
@@ -4025,7 +4031,7 @@
       <c r="F18" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="G18" s="77" t="s">
+      <c r="G18" s="60" t="s">
         <v>434</v>
       </c>
       <c r="J18" s="9" t="s">
@@ -4034,7 +4040,7 @@
       <c r="K18" s="24" t="s">
         <v>182</v>
       </c>
-      <c r="L18" s="77" t="s">
+      <c r="L18" s="60" t="s">
         <v>441</v>
       </c>
       <c r="M18" s="24" t="s">
@@ -4063,7 +4069,7 @@
       <c r="F19" s="6" t="s">
         <v>276</v>
       </c>
-      <c r="G19" s="77" t="s">
+      <c r="G19" s="60" t="s">
         <v>276</v>
       </c>
       <c r="J19" s="13" t="s">
@@ -4072,7 +4078,7 @@
       <c r="K19" s="24" t="s">
         <v>183</v>
       </c>
-      <c r="L19" s="77" t="s">
+      <c r="L19" s="60" t="s">
         <v>442</v>
       </c>
       <c r="M19" s="24" t="s">
@@ -4098,7 +4104,7 @@
       <c r="F20" s="21" t="s">
         <v>273</v>
       </c>
-      <c r="G20" s="77" t="s">
+      <c r="G20" s="60" t="s">
         <v>273</v>
       </c>
       <c r="J20" s="9" t="s">
@@ -4107,7 +4113,7 @@
       <c r="K20" s="24" t="s">
         <v>184</v>
       </c>
-      <c r="L20" s="77" t="s">
+      <c r="L20" s="60" t="s">
         <v>443</v>
       </c>
       <c r="M20" s="24" t="s">
@@ -4133,7 +4139,7 @@
       <c r="F21" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="G21" s="78" t="s">
+      <c r="G21" s="61" t="s">
         <v>444</v>
       </c>
       <c r="J21" s="9" t="s">
@@ -4171,7 +4177,7 @@
       <c r="F22" s="29" t="s">
         <v>279</v>
       </c>
-      <c r="G22" s="77" t="s">
+      <c r="G22" s="60" t="s">
         <v>487</v>
       </c>
       <c r="J22" s="9" t="s">
@@ -4180,7 +4186,7 @@
       <c r="K22" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="L22" s="77" t="s">
+      <c r="L22" s="60" t="s">
         <v>445</v>
       </c>
       <c r="M22" s="24" t="s">
@@ -4206,7 +4212,7 @@
       <c r="F23" s="21" t="s">
         <v>277</v>
       </c>
-      <c r="G23" s="77" t="s">
+      <c r="G23" s="60" t="s">
         <v>277</v>
       </c>
       <c r="J23" s="9" t="s">
@@ -4215,7 +4221,7 @@
       <c r="K23" s="24" t="s">
         <v>187</v>
       </c>
-      <c r="L23" s="77" t="s">
+      <c r="L23" s="60" t="s">
         <v>446</v>
       </c>
       <c r="M23" s="24" t="s">
@@ -4241,7 +4247,7 @@
       <c r="F24" s="21" t="s">
         <v>272</v>
       </c>
-      <c r="G24" s="77" t="s">
+      <c r="G24" s="60" t="s">
         <v>272</v>
       </c>
       <c r="J24" s="9" t="s">
@@ -4250,7 +4256,7 @@
       <c r="K24" s="24" t="s">
         <v>188</v>
       </c>
-      <c r="L24" s="77" t="s">
+      <c r="L24" s="60" t="s">
         <v>447</v>
       </c>
       <c r="M24" s="24" t="s">
@@ -4276,7 +4282,7 @@
       <c r="F25" s="21" t="s">
         <v>388</v>
       </c>
-      <c r="G25" s="77" t="s">
+      <c r="G25" s="60" t="s">
         <v>388</v>
       </c>
       <c r="J25" s="9" t="s">
@@ -4285,7 +4291,7 @@
       <c r="K25" s="24" t="s">
         <v>189</v>
       </c>
-      <c r="L25" s="77" t="s">
+      <c r="L25" s="60" t="s">
         <v>448</v>
       </c>
       <c r="M25" s="24" t="s">
@@ -4311,7 +4317,7 @@
       <c r="F26" s="21" t="s">
         <v>316</v>
       </c>
-      <c r="G26" s="77" t="s">
+      <c r="G26" s="60" t="s">
         <v>316</v>
       </c>
       <c r="J26" s="9" t="s">
@@ -4320,7 +4326,7 @@
       <c r="K26" s="24" t="s">
         <v>190</v>
       </c>
-      <c r="L26" s="77" t="s">
+      <c r="L26" s="60" t="s">
         <v>449</v>
       </c>
       <c r="M26" s="24" t="s">
@@ -4346,7 +4352,7 @@
       <c r="F27" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="G27" s="77" t="s">
+      <c r="G27" s="60" t="s">
         <v>98</v>
       </c>
       <c r="J27" s="9" t="s">
@@ -4355,7 +4361,7 @@
       <c r="K27" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="L27" s="77" t="s">
+      <c r="L27" s="60" t="s">
         <v>450</v>
       </c>
       <c r="M27" s="24" t="s">
@@ -4379,7 +4385,7 @@
       <c r="F28" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="G28" s="78" t="s">
+      <c r="G28" s="61" t="s">
         <v>444</v>
       </c>
       <c r="J28" s="9" t="s">
@@ -4417,7 +4423,7 @@
       <c r="F29" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="G29" s="77" t="s">
+      <c r="G29" s="60" t="s">
         <v>492</v>
       </c>
       <c r="J29" s="36" t="s">
@@ -4426,7 +4432,7 @@
       <c r="K29" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="L29" s="77" t="s">
+      <c r="L29" s="60" t="s">
         <v>451</v>
       </c>
       <c r="M29" s="24" t="s">
@@ -4452,13 +4458,13 @@
       <c r="F30" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="G30" s="77" t="s">
+      <c r="G30" s="60" t="s">
         <v>229</v>
       </c>
       <c r="K30" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="L30" s="77" t="s">
+      <c r="L30" s="60" t="s">
         <v>452</v>
       </c>
       <c r="M30" s="24" t="s">
@@ -4481,7 +4487,7 @@
       <c r="F31" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="G31" s="78" t="s">
+      <c r="G31" s="61" t="s">
         <v>444</v>
       </c>
       <c r="K31" s="24" t="s">
@@ -4551,7 +4557,7 @@
       <c r="F33" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="G33" s="77" t="s">
+      <c r="G33" s="60" t="s">
         <v>229</v>
       </c>
       <c r="J33" s="9" t="s">
@@ -4560,7 +4566,7 @@
       <c r="K33" s="24" t="s">
         <v>346</v>
       </c>
-      <c r="L33" s="77" t="s">
+      <c r="L33" s="60" t="s">
         <v>457</v>
       </c>
       <c r="M33" s="24" t="s">
@@ -4583,7 +4589,7 @@
       <c r="F34" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="G34" s="77" t="s">
+      <c r="G34" s="60" t="s">
         <v>229</v>
       </c>
       <c r="J34" s="9" t="s">
@@ -4592,7 +4598,7 @@
       <c r="K34" s="24" t="s">
         <v>338</v>
       </c>
-      <c r="L34" s="77" t="s">
+      <c r="L34" s="60" t="s">
         <v>458</v>
       </c>
       <c r="M34" s="24" t="s">
@@ -4621,13 +4627,13 @@
       <c r="F35" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="G35" s="77" t="s">
+      <c r="G35" s="60" t="s">
         <v>454</v>
       </c>
       <c r="J35" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="L35" s="77" t="s">
+      <c r="L35" s="60" t="s">
         <v>459</v>
       </c>
       <c r="M35" s="24" t="s">
@@ -4656,7 +4662,7 @@
       <c r="F36" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="G36" s="77" t="s">
+      <c r="G36" s="60" t="s">
         <v>455</v>
       </c>
       <c r="J36" s="9" t="s">
@@ -4665,7 +4671,7 @@
       <c r="K36" s="24" t="s">
         <v>320</v>
       </c>
-      <c r="L36" s="77" t="s">
+      <c r="L36" s="60" t="s">
         <v>460</v>
       </c>
       <c r="M36" s="24" t="s">
@@ -4694,7 +4700,7 @@
       <c r="F37" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="G37" s="77" t="s">
+      <c r="G37" s="60" t="s">
         <v>456</v>
       </c>
       <c r="J37" s="9" t="s">
@@ -4703,7 +4709,7 @@
       <c r="K37" s="24" t="s">
         <v>324</v>
       </c>
-      <c r="L37" s="77" t="s">
+      <c r="L37" s="60" t="s">
         <v>461</v>
       </c>
       <c r="M37" s="24" t="s">
@@ -4729,13 +4735,13 @@
       <c r="F38" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="G38" s="77" t="s">
+      <c r="G38" s="60" t="s">
         <v>229</v>
       </c>
       <c r="J38" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="L38" s="77" t="s">
+      <c r="L38" s="60" t="s">
         <v>462</v>
       </c>
       <c r="M38" s="24" t="s">
@@ -4761,13 +4767,13 @@
       <c r="F39" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="G39" s="77" t="s">
+      <c r="G39" s="60" t="s">
         <v>493</v>
       </c>
       <c r="J39" s="36" t="s">
         <v>156</v>
       </c>
-      <c r="L39" s="77" t="s">
+      <c r="L39" s="60" t="s">
         <v>463</v>
       </c>
       <c r="M39" s="24" t="s">
@@ -4793,7 +4799,7 @@
       <c r="F40" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="G40" s="77" t="s">
+      <c r="G40" s="60" t="s">
         <v>491</v>
       </c>
       <c r="J40" s="32" t="s">
@@ -4802,7 +4808,7 @@
       <c r="K40" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="L40" s="77" t="s">
+      <c r="L40" s="60" t="s">
         <v>464</v>
       </c>
       <c r="M40" s="24" t="s">
@@ -4826,7 +4832,7 @@
       <c r="F41" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="G41" s="78" t="s">
+      <c r="G41" s="61" t="s">
         <v>444</v>
       </c>
       <c r="J41" s="9" t="s">
@@ -4864,7 +4870,7 @@
       <c r="F42" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="G42" s="77" t="s">
+      <c r="G42" s="60" t="s">
         <v>502</v>
       </c>
       <c r="J42" s="9" t="s">
@@ -4873,7 +4879,7 @@
       <c r="K42" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="L42" s="79" t="s">
+      <c r="L42" s="62" t="s">
         <v>453</v>
       </c>
       <c r="M42" s="24" t="s">
@@ -4899,7 +4905,7 @@
       <c r="F43" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="G43" s="77" t="s">
+      <c r="G43" s="60" t="s">
         <v>465</v>
       </c>
       <c r="J43" s="9" t="s">
@@ -4908,7 +4914,7 @@
       <c r="K43" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="L43" s="77" t="s">
+      <c r="L43" s="60" t="s">
         <v>466</v>
       </c>
       <c r="M43" s="24" t="s">
@@ -4937,7 +4943,7 @@
       <c r="F44" s="21" t="s">
         <v>276</v>
       </c>
-      <c r="G44" s="77" t="s">
+      <c r="G44" s="60" t="s">
         <v>276</v>
       </c>
       <c r="J44" s="53" t="s">
@@ -4946,7 +4952,7 @@
       <c r="K44" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="L44" s="77" t="s">
+      <c r="L44" s="60" t="s">
         <v>467</v>
       </c>
       <c r="M44" s="24" t="s">
@@ -4972,7 +4978,7 @@
       <c r="F45" s="29" t="s">
         <v>359</v>
       </c>
-      <c r="G45" s="77" t="s">
+      <c r="G45" s="60" t="s">
         <v>494</v>
       </c>
       <c r="J45" s="9" t="s">
@@ -4981,7 +4987,7 @@
       <c r="K45" s="24" t="s">
         <v>377</v>
       </c>
-      <c r="L45" s="80" t="s">
+      <c r="L45" s="63" t="s">
         <v>490</v>
       </c>
       <c r="M45" s="24" t="s">
@@ -5007,7 +5013,7 @@
       <c r="F46" s="29" t="s">
         <v>360</v>
       </c>
-      <c r="G46" s="77" t="s">
+      <c r="G46" s="60" t="s">
         <v>495</v>
       </c>
       <c r="J46" s="9" t="s">
@@ -5016,7 +5022,7 @@
       <c r="K46" s="24" t="s">
         <v>378</v>
       </c>
-      <c r="L46" s="77" t="s">
+      <c r="L46" s="60" t="s">
         <v>468</v>
       </c>
       <c r="M46" s="24" t="s">
@@ -5042,7 +5048,7 @@
       <c r="F47" s="29" t="s">
         <v>388</v>
       </c>
-      <c r="G47" s="77" t="s">
+      <c r="G47" s="60" t="s">
         <v>388</v>
       </c>
       <c r="J47" s="9" t="s">
@@ -5051,7 +5057,7 @@
       <c r="K47" s="24" t="s">
         <v>379</v>
       </c>
-      <c r="L47" s="77" t="s">
+      <c r="L47" s="60" t="s">
         <v>469</v>
       </c>
       <c r="M47" s="24" t="s">
@@ -5077,7 +5083,7 @@
       <c r="F48" s="29" t="s">
         <v>374</v>
       </c>
-      <c r="G48" s="77" t="s">
+      <c r="G48" s="60" t="s">
         <v>496</v>
       </c>
       <c r="J48" s="9" t="s">
@@ -5086,7 +5092,7 @@
       <c r="K48" s="24" t="s">
         <v>380</v>
       </c>
-      <c r="L48" s="77" t="s">
+      <c r="L48" s="60" t="s">
         <v>470</v>
       </c>
       <c r="M48" s="24" t="s">
@@ -5112,7 +5118,7 @@
       <c r="F49" s="29" t="s">
         <v>361</v>
       </c>
-      <c r="G49" s="77" t="s">
+      <c r="G49" s="60" t="s">
         <v>497</v>
       </c>
       <c r="J49" s="9" t="s">
@@ -5121,7 +5127,7 @@
       <c r="K49" s="24" t="s">
         <v>381</v>
       </c>
-      <c r="L49" s="77" t="s">
+      <c r="L49" s="60" t="s">
         <v>471</v>
       </c>
       <c r="M49" s="24" t="s">
@@ -5147,7 +5153,7 @@
       <c r="F50" s="29" t="s">
         <v>362</v>
       </c>
-      <c r="G50" s="77" t="s">
+      <c r="G50" s="60" t="s">
         <v>498</v>
       </c>
       <c r="J50" s="9" t="s">
@@ -5156,7 +5162,7 @@
       <c r="K50" s="24" t="s">
         <v>392</v>
       </c>
-      <c r="L50" s="77" t="s">
+      <c r="L50" s="60" t="s">
         <v>472</v>
       </c>
       <c r="M50" s="24" t="s">
@@ -5182,7 +5188,7 @@
       <c r="F51" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="G51" s="77" t="s">
+      <c r="G51" s="60" t="s">
         <v>492</v>
       </c>
       <c r="J51" s="32" t="s">
@@ -5191,7 +5197,7 @@
       <c r="K51" s="24" t="s">
         <v>382</v>
       </c>
-      <c r="L51" s="77" t="s">
+      <c r="L51" s="60" t="s">
         <v>473</v>
       </c>
       <c r="M51" s="24" t="s">
@@ -5217,7 +5223,7 @@
       <c r="F52" s="29" t="s">
         <v>362</v>
       </c>
-      <c r="G52" s="77" t="s">
+      <c r="G52" s="60" t="s">
         <v>498</v>
       </c>
       <c r="J52" s="9" t="s">
@@ -5226,7 +5232,7 @@
       <c r="K52" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="L52" s="77" t="s">
+      <c r="L52" s="60" t="s">
         <v>474</v>
       </c>
       <c r="M52" s="24" t="s">
@@ -5252,7 +5258,7 @@
       <c r="F53" s="29" t="s">
         <v>207</v>
       </c>
-      <c r="G53" s="77" t="s">
+      <c r="G53" s="60" t="s">
         <v>499</v>
       </c>
       <c r="J53" s="9" t="s">
@@ -5261,7 +5267,7 @@
       <c r="K53" s="24" t="s">
         <v>383</v>
       </c>
-      <c r="L53" s="77" t="s">
+      <c r="L53" s="60" t="s">
         <v>475</v>
       </c>
       <c r="M53" s="24" t="s">
@@ -5287,7 +5293,7 @@
       <c r="F54" s="29" t="s">
         <v>363</v>
       </c>
-      <c r="G54" s="77" t="s">
+      <c r="G54" s="60" t="s">
         <v>500</v>
       </c>
       <c r="J54" s="32" t="s">
@@ -5296,7 +5302,7 @@
       <c r="K54" s="24" t="s">
         <v>384</v>
       </c>
-      <c r="L54" s="77" t="s">
+      <c r="L54" s="60" t="s">
         <v>476</v>
       </c>
       <c r="M54" s="24" t="s">
@@ -5322,7 +5328,7 @@
       <c r="F55" s="29" t="s">
         <v>363</v>
       </c>
-      <c r="G55" s="77" t="s">
+      <c r="G55" s="60" t="s">
         <v>500</v>
       </c>
       <c r="J55" s="9" t="s">
@@ -5331,7 +5337,7 @@
       <c r="K55" s="24" t="s">
         <v>385</v>
       </c>
-      <c r="L55" s="77" t="s">
+      <c r="L55" s="60" t="s">
         <v>477</v>
       </c>
       <c r="M55" s="24" t="s">
@@ -5357,7 +5363,7 @@
       <c r="F56" s="29" t="s">
         <v>373</v>
       </c>
-      <c r="G56" s="77" t="s">
+      <c r="G56" s="60" t="s">
         <v>501</v>
       </c>
       <c r="J56" s="9" t="s">
@@ -5366,7 +5372,7 @@
       <c r="K56" s="24" t="s">
         <v>386</v>
       </c>
-      <c r="L56" s="77" t="s">
+      <c r="L56" s="60" t="s">
         <v>478</v>
       </c>
       <c r="M56" s="24" t="s">
@@ -5392,7 +5398,7 @@
       <c r="F57" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="G57" s="78" t="s">
+      <c r="G57" s="61" t="s">
         <v>444</v>
       </c>
       <c r="J57" s="9" t="s">
@@ -5427,7 +5433,7 @@
       <c r="E58" s="59" t="s">
         <v>334</v>
       </c>
-      <c r="F58" s="77" t="s">
+      <c r="F58" s="60" t="s">
         <v>229</v>
       </c>
       <c r="G58" s="21" t="s">
@@ -5439,7 +5445,7 @@
       <c r="K58" s="24" t="s">
         <v>337</v>
       </c>
-      <c r="L58" s="77" t="s">
+      <c r="L58" s="60" t="s">
         <v>6</v>
       </c>
       <c r="M58" s="24" t="s">
@@ -5450,56 +5456,56 @@
       </c>
     </row>
     <row r="59" spans="1:15" ht="29" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="81" t="s">
+      <c r="A59" s="64" t="s">
         <v>416</v>
       </c>
       <c r="B59" s="28" t="s">
         <v>417</v>
       </c>
-      <c r="D59" s="81" t="s">
+      <c r="D59" s="64" t="s">
         <v>418</v>
       </c>
-      <c r="G59" s="77" t="s">
+      <c r="G59" s="60" t="s">
         <v>276</v>
       </c>
       <c r="J59" s="53" t="s">
         <v>210</v>
       </c>
-      <c r="L59" s="77" t="s">
+      <c r="L59" s="60" t="s">
         <v>419</v>
       </c>
     </row>
     <row r="60" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="77" t="s">
+      <c r="A60" s="60" t="s">
         <v>479</v>
       </c>
-      <c r="D60" s="77" t="s">
+      <c r="D60" s="60" t="s">
         <v>481</v>
       </c>
-      <c r="G60" s="77" t="s">
+      <c r="G60" s="60" t="s">
         <v>488</v>
       </c>
       <c r="J60" s="31" t="s">
         <v>485</v>
       </c>
-      <c r="L60" s="77" t="s">
+      <c r="L60" s="60" t="s">
         <v>483</v>
       </c>
     </row>
     <row r="61" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="77" t="s">
+      <c r="A61" s="60" t="s">
         <v>480</v>
       </c>
-      <c r="D61" s="77" t="s">
+      <c r="D61" s="60" t="s">
         <v>482</v>
       </c>
-      <c r="G61" s="77" t="s">
+      <c r="G61" s="60" t="s">
         <v>489</v>
       </c>
       <c r="J61" s="31" t="s">
         <v>486</v>
       </c>
-      <c r="L61" s="77" t="s">
+      <c r="L61" s="60" t="s">
         <v>484</v>
       </c>
     </row>
@@ -5526,16 +5532,24 @@
         <v>358</v>
       </c>
     </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A63" s="57" t="s">
+        <v>510</v>
+      </c>
+      <c r="L63" s="50" t="s">
+        <v>511</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="A1:E1"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>